<commit_message>
thinh commit toi 24.12
</commit_message>
<xml_diff>
--- a/INDRUINO_SOFT/IPQC_CHECKING_SYSTEM/bin/Debug/DATABASE.xlsx
+++ b/INDRUINO_SOFT/IPQC_CHECKING_SYSTEM/bin/Debug/DATABASE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IPQC-CHECKING-SYSTEM-master\INDRUINO_SOFT\IPQC_CHECKING_SYSTEM\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SOURCEMOI\IPQC-CHECKING-SYSTEM-master\INDRUINO_SOFT\IPQC_CHECKING_SYSTEM\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3124EFEC-73B1-4DDD-B909-445C4E4CF6E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03B55BC9-6921-4DE0-9AF6-E7B6F5596A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBD71C6F-1F8F-40FF-97D6-A5D11A5269D7}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" xr2:uid="{DBD71C6F-1F8F-40FF-97D6-A5D11A5269D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>PART CODE</t>
   </si>
@@ -88,6 +88,54 @@
   </si>
   <si>
     <t>10 H 42</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>3 H 18</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Repair</t>
+  </si>
+  <si>
+    <t>3 H 19</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>sdsa</t>
+  </si>
+  <si>
+    <t>3 H 20</t>
+  </si>
+  <si>
+    <t>3 H 23</t>
+  </si>
+  <si>
+    <t>3 H 24</t>
+  </si>
+  <si>
+    <t>as</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>3 H 29</t>
+  </si>
+  <si>
+    <t>3 H 30</t>
   </si>
 </sst>
 </file>
@@ -456,18 +504,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA864F39-6149-4289-9D68-FA8185B3E3E1}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -552,6 +600,219 @@
         <v>18</v>
       </c>
     </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Thinh comimit vs 25.12.2019
</commit_message>
<xml_diff>
--- a/INDRUINO_SOFT/IPQC_CHECKING_SYSTEM/bin/Debug/DATABASE.xlsx
+++ b/INDRUINO_SOFT/IPQC_CHECKING_SYSTEM/bin/Debug/DATABASE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SOURCEMOI\IPQC-CHECKING-SYSTEM-master\INDRUINO_SOFT\IPQC_CHECKING_SYSTEM\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2019\IPQC CHECKING\IPQC-CHECKING-SYSTEM\INDRUINO_SOFT\IPQC_CHECKING_SYSTEM\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03B55BC9-6921-4DE0-9AF6-E7B6F5596A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E142B081-F078-428C-B373-375A02800148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="15375" windowHeight="7875" xr2:uid="{DBD71C6F-1F8F-40FF-97D6-A5D11A5269D7}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{DBD71C6F-1F8F-40FF-97D6-A5D11A5269D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>PART CODE</t>
   </si>
@@ -102,9 +102,6 @@
     <t>NG</t>
   </si>
   <si>
-    <t>T</t>
-  </si>
-  <si>
     <t>Repair</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>3 H 30</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -634,16 +634,13 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="L4" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -655,10 +652,10 @@
         <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -667,12 +664,18 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -684,16 +687,16 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
-        <v>29</v>
-      </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -703,17 +706,14 @@
       </c>
       <c r="K6" t="s">
         <v>22</v>
-      </c>
-      <c r="L6" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>20</v>
@@ -722,13 +722,13 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -737,33 +737,39 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>33</v>
-      </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -773,35 +779,29 @@
       </c>
       <c r="K8" t="s">
         <v>22</v>
-      </c>
-      <c r="L8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M8" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>33</v>
       </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -810,7 +810,13 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>